<commit_message>
fixing entites report content
</commit_message>
<xml_diff>
--- a/reports/Menu.xlsx
+++ b/reports/Menu.xlsx
@@ -17,6 +17,120 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> U R L</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Icon U R L</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Font   Color</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Background Color</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I D</t>
+  </si>
+  <si>
+    <t>user_role</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> User Role</t>
+  </si>
+  <si>
+    <t>Generated Management Page for: UserRole</t>
+  </si>
+  <si>
+    <t>/management/user_role</t>
+  </si>
+  <si>
+    <t>&amp;{&lt;nil&gt; {725 2020-08-04 13:29:28 +0700 +07 2020-08-08 13:52:43 +0700 +07 &lt;nil&gt;} management Management 1 0 /page/management [Generated] Management Page  1 []}</t>
+  </si>
+  <si>
+    <t>DefaultIcon.bmp</t>
+  </si>
+  <si>
+    <t>#000000</t>
+  </si>
+  <si>
+    <t>#ffffff</t>
+  </si>
+  <si>
+    <t>page</t>
+  </si>
+  <si>
+    <t>Generated Management Page for: Page</t>
+  </si>
+  <si>
+    <t>/management/page</t>
+  </si>
+  <si>
+    <t>profile</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Profile</t>
+  </si>
+  <si>
+    <t>Generated Management Page for: Profile</t>
+  </si>
+  <si>
+    <t>/management/profile</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>HOME</t>
+  </si>
+  <si>
+    <t>Generated [home]</t>
+  </si>
+  <si>
+    <t>/admin/home</t>
+  </si>
+  <si>
+    <t>&amp;{&lt;nil&gt; {723 2020-08-04 13:29:28 +0700 +07 2020-08-08 13:52:42 +0700 +07 &lt;nil&gt;} admin Admin 1 0 /page/admin [Generated] Admin Page  0 []}</t>
+  </si>
+  <si>
+    <t>pagesettings</t>
+  </si>
+  <si>
+    <t>PAGESETTINGS</t>
+  </si>
+  <si>
+    <t>Generated [pagesettings]</t>
+  </si>
+  <si>
+    <t>/admin/pagesettings</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> User</t>
+  </si>
+  <si>
+    <t>Generated Management Page for: User</t>
+  </si>
+  <si>
+    <t>/management/user</t>
+  </si>
+  <si>
     <t>registered_request</t>
   </si>
   <si>
@@ -29,18 +143,6 @@
     <t>/management/registered_request</t>
   </si>
   <si>
-    <t>&amp;{&lt;nil&gt; {725 2020-08-04 13:29:28 +0700 +07 2020-08-08 13:52:43 +0700 +07 &lt;nil&gt;} management Management 1 0 /page/management [Generated] Management Page  1 []}</t>
-  </si>
-  <si>
-    <t>DefaultIcon.bmp</t>
-  </si>
-  <si>
-    <t>#000000</t>
-  </si>
-  <si>
-    <t>#ffffff</t>
-  </si>
-  <si>
     <t>menu</t>
   </si>
   <si>
@@ -51,108 +153,6 @@
   </si>
   <si>
     <t>/management/menu</t>
-  </si>
-  <si>
-    <t>page</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Page</t>
-  </si>
-  <si>
-    <t>Generated Management Page for: Page</t>
-  </si>
-  <si>
-    <t>/management/page</t>
-  </si>
-  <si>
-    <t>profile</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Profile</t>
-  </si>
-  <si>
-    <t>Generated Management Page for: Profile</t>
-  </si>
-  <si>
-    <t>/management/profile</t>
-  </si>
-  <si>
-    <t>user</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> User</t>
-  </si>
-  <si>
-    <t>Generated Management Page for: User</t>
-  </si>
-  <si>
-    <t>/management/user</t>
-  </si>
-  <si>
-    <t>home</t>
-  </si>
-  <si>
-    <t>HOME</t>
-  </si>
-  <si>
-    <t>Generated [home]</t>
-  </si>
-  <si>
-    <t>/admin/home</t>
-  </si>
-  <si>
-    <t>&amp;{&lt;nil&gt; {723 2020-08-04 13:29:28 +0700 +07 2020-08-08 13:52:42 +0700 +07 &lt;nil&gt;} admin Admin 1 0 /page/admin [Generated] Admin Page  0 []}</t>
-  </si>
-  <si>
-    <t>pagesettings</t>
-  </si>
-  <si>
-    <t>PAGESETTINGS</t>
-  </si>
-  <si>
-    <t>Generated [pagesettings]</t>
-  </si>
-  <si>
-    <t>/admin/pagesettings</t>
-  </si>
-  <si>
-    <t>user_role</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> User Role</t>
-  </si>
-  <si>
-    <t>Generated Management Page for: UserRole</t>
-  </si>
-  <si>
-    <t>/management/user_role</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> U R L</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Icon U R L</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Font   Color</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Background Color</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> I D</t>
   </si>
 </sst>
 </file>
@@ -481,34 +481,34 @@
     <row r="1"/>
     <row r="2">
       <c r="C2" t="s">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="I2" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="J2" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="K2" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="L2" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
@@ -516,28 +516,28 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I3" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="J3" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="K3" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="L3">
         <v>1092</v>
@@ -548,28 +548,28 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" t="s">
         <v>29</v>
       </c>
-      <c r="E4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" t="s">
-        <v>28</v>
-      </c>
       <c r="I4" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="J4" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="K4" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="L4">
         <v>1093</v>
@@ -580,28 +580,28 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="H5" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="I5" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="J5" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="K5" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="L5">
         <v>1094</v>
@@ -612,28 +612,28 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="H6" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="I6" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="J6" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="K6" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="L6">
         <v>1095</v>
@@ -644,28 +644,28 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="F7" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="G7" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="H7" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="I7" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="J7" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="K7" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="L7">
         <v>1096</v>
@@ -676,28 +676,28 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="E8" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="G8" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="H8" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="I8" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="J8" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="K8" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="L8">
         <v>1097</v>
@@ -708,28 +708,28 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" t="s">
         <v>14</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I9" t="s">
         <v>15</v>
       </c>
-      <c r="H9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I9" t="s">
-        <v>5</v>
-      </c>
       <c r="J9" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="K9" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="L9">
         <v>1098</v>
@@ -740,28 +740,28 @@
         <v>8</v>
       </c>
       <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" t="s">
         <v>16</v>
       </c>
-      <c r="E10" t="s">
+      <c r="K10" t="s">
         <v>17</v>
-      </c>
-      <c r="F10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10" t="s">
-        <v>4</v>
-      </c>
-      <c r="I10" t="s">
-        <v>5</v>
-      </c>
-      <c r="J10" t="s">
-        <v>6</v>
-      </c>
-      <c r="K10" t="s">
-        <v>7</v>
       </c>
       <c r="L10">
         <v>1099</v>

</xml_diff>